<commit_message>
Se agrega carpeta nueva
</commit_message>
<xml_diff>
--- a/Taller_R_uces_2_2019/08_26_Tidy_2/datosLong1.xlsx
+++ b/Taller_R_uces_2_2019/08_26_Tidy_2/datosLong1.xlsx
@@ -1,77 +1,84 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pabloandres/Documents/OneDrive/TalleresCursos/Taller_R_uces_2_2019/08_26_Tidy_2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_FCC7368AAF6469224F3A7C5AE9A8FB96E3CDF4B8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22020" windowHeight="11200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="metadatos" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="datos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="metadatos" sheetId="1" r:id="rId1"/>
+    <sheet name="datos" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sexo_trat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">masc-a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">masc-b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fem-a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fem-b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción de las variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">descripción</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identificación única de cada sujeto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Género (fem ó masc) de cada sujeto en conjunto con el tratamiento asigando (a ó b)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Respuesta medida en el tiempo 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Respuesta medida en el tiempo 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Respuesta medida en el tiempo 3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>sexo_trat</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>masc-a</t>
+  </si>
+  <si>
+    <t>masc-b</t>
+  </si>
+  <si>
+    <t>fem-a</t>
+  </si>
+  <si>
+    <t>fem-b</t>
+  </si>
+  <si>
+    <t>Descripción de las variables</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>descripción</t>
+  </si>
+  <si>
+    <t>Identificación única de cada sujeto</t>
+  </si>
+  <si>
+    <t>Género (fem ó masc) de cada sujeto en conjunto con el tratamiento asigando (a ó b)</t>
+  </si>
+  <si>
+    <t>Respuesta medida en el tiempo 1</t>
+  </si>
+  <si>
+    <t>Respuesta medida en el tiempo 2</t>
+  </si>
+  <si>
+    <t>Respuesta medida en el tiempo 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -85,10 +92,10 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <i/>
     </font>
   </fonts>
   <fills count="3">
@@ -116,53 +123,81 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -186,6 +221,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -467,19 +511,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -487,7 +531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -495,7 +539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -503,7 +547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -511,7 +555,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -519,7 +563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -529,19 +573,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="C4:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -558,518 +604,518 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="C5" s="1" t="n">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" s="1">
         <v>31</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="4">
         <v>51.02</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="4">
         <v>67.83</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="6">
         <v>82.87</v>
       </c>
     </row>
-    <row r="6">
-      <c r="C6" s="2" t="n">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="2">
         <v>52</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>40.18</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>49.39</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="7">
         <v>72.94</v>
       </c>
     </row>
-    <row r="7">
-      <c r="C7" s="2" t="n">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="2">
         <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>51.7</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>72.63</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="G7" s="7">
         <v>56.73</v>
       </c>
     </row>
-    <row r="8">
-      <c r="C8" s="2" t="n">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="2">
         <v>39</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>43.33</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>62.1</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="7">
         <v>69.19</v>
       </c>
     </row>
-    <row r="9">
-      <c r="C9" s="2" t="n">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="2">
         <v>48</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>67.17</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>56.33</v>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="G9" s="7">
         <v>53.56</v>
       </c>
     </row>
-    <row r="10">
-      <c r="C10" s="2" t="n">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="2">
         <v>60</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>57.22</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>54.31</v>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="G10" s="7">
         <v>80.25</v>
       </c>
     </row>
-    <row r="11">
-      <c r="C11" s="2" t="n">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C11" s="2">
         <v>40</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>54.89</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>45.7</v>
       </c>
-      <c r="G11" s="7" t="n">
+      <c r="G11" s="7">
         <v>64.17</v>
       </c>
     </row>
-    <row r="12">
-      <c r="C12" s="2" t="n">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C12" s="2">
         <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" t="n">
-        <v>36.27</v>
-      </c>
-      <c r="F12" t="n">
+      <c r="E12">
+        <v>36.270000000000003</v>
+      </c>
+      <c r="F12">
         <v>36.06</v>
       </c>
-      <c r="G12" s="7" t="n">
+      <c r="G12" s="7">
         <v>62.89</v>
       </c>
     </row>
-    <row r="13">
-      <c r="C13" s="2" t="n">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C13" s="2">
         <v>14</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>55.85</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>57.28</v>
       </c>
-      <c r="G13" s="7" t="n">
-        <v>69.68</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="2" t="n">
+      <c r="G13" s="7">
+        <v>69.680000000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C14" s="2">
         <v>43</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>39.9</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>75.06</v>
       </c>
-      <c r="G14" s="7" t="n">
+      <c r="G14" s="7">
         <v>60.06</v>
       </c>
     </row>
-    <row r="15">
-      <c r="C15" s="2" t="n">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C15" s="2">
         <v>58</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>47.87</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>60.81</v>
       </c>
-      <c r="G15" s="7" t="n">
-        <v>74.9</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" s="2" t="n">
+      <c r="G15" s="7">
+        <v>74.900000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C16" s="2">
         <v>30</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>73.92</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>57.5</v>
       </c>
-      <c r="G16" s="7" t="n">
+      <c r="G16" s="7">
         <v>77.11</v>
       </c>
     </row>
-    <row r="17">
-      <c r="C17" s="2" t="n">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C17" s="2">
         <v>59</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>50.86</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>50.65</v>
       </c>
-      <c r="G17" s="7" t="n">
+      <c r="G17" s="7">
         <v>77.02</v>
       </c>
     </row>
-    <row r="18">
-      <c r="C18" s="2" t="n">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C18" s="2">
         <v>9</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>57.57</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>50.92</v>
       </c>
-      <c r="G18" s="7" t="n">
+      <c r="G18" s="7">
         <v>70.19</v>
       </c>
     </row>
-    <row r="19">
-      <c r="C19" s="2" t="n">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C19" s="2">
         <v>56</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>51.53</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>52.56</v>
       </c>
-      <c r="G19" s="7" t="n">
+      <c r="G19" s="7">
         <v>71.67</v>
       </c>
     </row>
-    <row r="20">
-      <c r="C20" s="2" t="n">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C20" s="2">
         <v>16</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>61.37</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>62.44</v>
       </c>
-      <c r="G20" s="7" t="n">
+      <c r="G20" s="7">
         <v>66.23</v>
       </c>
     </row>
-    <row r="21">
-      <c r="C21" s="2" t="n">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C21" s="2">
         <v>22</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>43.58</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>59.01</v>
       </c>
-      <c r="G21" s="7" t="n">
+      <c r="G21" s="7">
         <v>61.27</v>
       </c>
     </row>
-    <row r="22">
-      <c r="C22" s="2" t="n">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C22" s="2">
         <v>41</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>53.56</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22">
         <v>57.67</v>
       </c>
-      <c r="G22" s="7" t="n">
+      <c r="G22" s="7">
         <v>59.87</v>
       </c>
     </row>
-    <row r="23">
-      <c r="C23" s="2" t="n">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C23" s="2">
         <v>5</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>39.96</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>54.69</v>
       </c>
-      <c r="G23" s="7" t="n">
+      <c r="G23" s="7">
         <v>55.54</v>
       </c>
     </row>
-    <row r="24">
-      <c r="C24" s="2" t="n">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C24" s="2">
         <v>55</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>63.88</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24">
         <v>52.42</v>
       </c>
-      <c r="G24" s="7" t="n">
+      <c r="G24" s="7">
         <v>69.3</v>
       </c>
     </row>
-    <row r="25">
-      <c r="C25" s="2" t="n">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C25" s="2">
         <v>15</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>42.21</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25">
         <v>64.13</v>
       </c>
-      <c r="G25" s="7" t="n">
+      <c r="G25" s="7">
         <v>54.3</v>
       </c>
     </row>
-    <row r="26">
-      <c r="C26" s="2" t="n">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C26" s="2">
         <v>10</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26">
         <v>30.97</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26">
         <v>52.16</v>
       </c>
-      <c r="G26" s="7" t="n">
+      <c r="G26" s="7">
         <v>54.1</v>
       </c>
     </row>
-    <row r="27">
-      <c r="C27" s="2" t="n">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C27" s="2">
         <v>28</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27">
         <v>42.16</v>
       </c>
-      <c r="F27" t="n">
+      <c r="F27">
         <v>64.91</v>
       </c>
-      <c r="G27" s="7" t="n">
+      <c r="G27" s="7">
         <v>56.32</v>
       </c>
     </row>
-    <row r="28">
-      <c r="C28" s="2" t="n">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C28" s="2">
         <v>33</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
-      <c r="E28" t="n">
+      <c r="E28">
         <v>57.93</v>
       </c>
-      <c r="F28" t="n">
+      <c r="F28">
         <v>54.47</v>
       </c>
-      <c r="G28" s="7" t="n">
+      <c r="G28" s="7">
         <v>60.82</v>
       </c>
     </row>
-    <row r="29">
-      <c r="C29" s="2" t="n">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C29" s="2">
         <v>37</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E29">
         <v>56.01</v>
       </c>
-      <c r="F29" t="n">
+      <c r="F29">
         <v>51.76</v>
       </c>
-      <c r="G29" s="7" t="n">
+      <c r="G29" s="7">
         <v>63.1</v>
       </c>
     </row>
-    <row r="30">
-      <c r="C30" s="2" t="n">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C30" s="2">
         <v>51</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E30">
         <v>61.04</v>
       </c>
-      <c r="F30" t="n">
+      <c r="F30">
         <v>73.27</v>
       </c>
-      <c r="G30" s="7" t="n">
+      <c r="G30" s="7">
         <v>67.64</v>
       </c>
     </row>
-    <row r="31">
-      <c r="C31" s="2" t="n">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C31" s="2">
         <v>38</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E31">
         <v>41.39</v>
       </c>
-      <c r="F31" t="n">
+      <c r="F31">
         <v>61.28</v>
       </c>
-      <c r="G31" s="7" t="n">
+      <c r="G31" s="7">
         <v>72.87</v>
       </c>
     </row>
-    <row r="32">
-      <c r="C32" s="2" t="n">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C32" s="2">
         <v>42</v>
       </c>
       <c r="D32" t="s">
         <v>5</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E32">
         <v>31.31</v>
       </c>
-      <c r="F32" t="n">
+      <c r="F32">
         <v>85.65</v>
       </c>
-      <c r="G32" s="7" t="n">
+      <c r="G32" s="7">
         <v>78.77</v>
       </c>
     </row>
-    <row r="33">
-      <c r="C33" s="2" t="n">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C33" s="2">
         <v>29</v>
       </c>
       <c r="D33" t="s">
         <v>8</v>
       </c>
-      <c r="E33" t="n">
-        <v>36.34</v>
-      </c>
-      <c r="F33" t="n">
+      <c r="E33">
+        <v>36.340000000000003</v>
+      </c>
+      <c r="F33">
         <v>52.46</v>
       </c>
-      <c r="G33" s="7" t="n">
+      <c r="G33" s="7">
         <v>67.5</v>
       </c>
     </row>
-    <row r="34">
-      <c r="C34" s="3" t="n">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34" s="3">
         <v>27</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="5" t="n">
+      <c r="E34" s="5">
         <v>41.64</v>
       </c>
-      <c r="F34" s="5" t="n">
+      <c r="F34" s="5">
         <v>38.67</v>
       </c>
-      <c r="G34" s="8" t="n">
+      <c r="G34" s="8">
         <v>56.61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>